<commit_message>
adding in acknowledgements table and updating gitignore
</commit_message>
<xml_diff>
--- a/data/mpox_tmrca.xlsx
+++ b/data/mpox_tmrca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mparedes/Desktop/gitrepos/monkeypox-dynamics-mp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{740CC612-04F0-3742-A8BB-2BD5E29B61CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BC3CF6-C47A-3E4C-A8FB-1311C963B138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{80AA68E8-77EA-CF41-B0DF-EC6E51C47CFA}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,5 +608,6 @@
     <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>